<commit_message>
Fixed index bug. Tests pass
</commit_message>
<xml_diff>
--- a/Tests/Sample.xlsx
+++ b/Tests/Sample.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -20,6 +20,12 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
   <si>
     <t>bla 1</t>
@@ -115,11 +121,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -127,68 +133,79 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
         <v>7.0</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed the need to specify type in excel file
</commit_message>
<xml_diff>
--- a/Tests/Sample.xlsx
+++ b/Tests/Sample.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -20,12 +20,6 @@
   </si>
   <si>
     <t>Location</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>String</t>
   </si>
   <si>
     <t>bla 1</t>
@@ -1229,7 +1223,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1257,11 +1251,11 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>3</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>4</v>
       </c>
       <c r="C2" t="s" s="2">
         <v>4</v>
@@ -1271,7 +1265,7 @@
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s" s="2">
         <v>5</v>
@@ -1284,77 +1278,71 @@
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s" s="2">
         <v>7</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="2">
         <v>9</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>6</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s" s="2">
         <v>10</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>6</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>4</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="4">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s" s="2">
-        <v>6</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
@@ -1372,13 +1360,6 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" ht="13.65" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>